<commit_message>
Bug Fixing and Added new Components
</commit_message>
<xml_diff>
--- a/src/frontend/src/assets/samples/sampleUpload.xlsx
+++ b/src/frontend/src/assets/samples/sampleUpload.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>S. No.</t>
   </si>
@@ -142,13 +142,125 @@
   </si>
   <si>
     <t>The first state in the country to apply 'Web based learning program' on December 23, 2014 is</t>
+  </si>
+  <si>
+    <t>QUESTION TEXT HINDI</t>
+  </si>
+  <si>
+    <r>
+      <t>निम्न में से किस बैंक की शाखाएं सबसे ज्यादा हैं</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">? </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">नैशनल स्टॉक एक्सचेंज स्थित है </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>विश्व बैंक का का मुख्यालय कहाँ है</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">? </t>
+    </r>
+  </si>
+  <si>
+    <t>OPTION1 HINDI</t>
+  </si>
+  <si>
+    <t>OPTION2 HINDI</t>
+  </si>
+  <si>
+    <t>OPTION3 HINDI</t>
+  </si>
+  <si>
+    <t>OPTION4 HINDI</t>
+  </si>
+  <si>
+    <t>OPTION5 HINDI</t>
+  </si>
+  <si>
+    <t>OPTION6 HINDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">इलाहाबाद बैंक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">नई दिल्ली </t>
+  </si>
+  <si>
+    <t xml:space="preserve">अमेरिका </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> एच० डी० एफ० सी० बैंक </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> मुम्बई </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> लन्दन </t>
+  </si>
+  <si>
+    <t xml:space="preserve">आई० सी० आई० सी० आई० बैंक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">कोलकाता </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">वाशिंगटन </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">DC </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">भारतीय स्टेट बैंक </t>
+  </si>
+  <si>
+    <t xml:space="preserve">बैंगलोर </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> न्यूयार्क </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +270,16 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lohit Devanagari"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -198,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -207,6 +329,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,20 +627,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" customWidth="1"/>
+    <col min="20" max="20" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="39">
+    <row r="1" spans="1:22" ht="39">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,170 +651,243 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="R1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:22" ht="39">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="3"/>
+      <c r="V2" s="3"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:22">
       <c r="A3" s="3">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="L3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="3"/>
+      <c r="V3" s="3"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:22" ht="26.25">
       <c r="A4" s="3">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="L4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="3"/>
+      <c r="V4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>